<commit_message>
with addition of memorial day and washington's bday holidays
</commit_message>
<xml_diff>
--- a/2021_cboc_signin_sheets/12December_2021_cboc_signin_sheet.xlsx
+++ b/2021_cboc_signin_sheets/12December_2021_cboc_signin_sheet.xlsx
@@ -2522,8 +2522,8 @@
     <col customWidth="1" max="29" min="29" width="4.5"/>
     <col customWidth="1" max="30" min="30" width="4.5"/>
     <col customWidth="1" max="31" min="31" width="4.5"/>
-    <col customWidth="1" max="32" min="32" width="4.5"/>
-    <col customWidth="1" max="33" min="33" width="4.5"/>
+    <col customWidth="1" max="32" min="32" width="2.5"/>
+    <col customWidth="1" max="33" min="33" width="2.5"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="45" r="1">
@@ -2661,12 +2661,12 @@
         </is>
       </c>
       <c r="AE2" s="6" t="n"/>
-      <c r="AF2" s="5" t="inlineStr">
+      <c r="AF2" s="7" t="inlineStr">
         <is>
           <t>FRI</t>
         </is>
       </c>
-      <c r="AG2" s="6" t="n"/>
+      <c r="AG2" s="8" t="n"/>
     </row>
     <row customHeight="1" ht="22" r="3">
       <c r="A3" s="9" t="inlineStr">
@@ -2734,10 +2734,10 @@
         <v>30</v>
       </c>
       <c r="AE3" s="6" t="n"/>
-      <c r="AF3" s="5" t="n">
+      <c r="AF3" s="7" t="n">
         <v>31</v>
       </c>
-      <c r="AG3" s="6" t="n"/>
+      <c r="AG3" s="8" t="n"/>
     </row>
     <row customHeight="1" ht="27" r="4">
       <c r="A4" s="10" t="n"/>
@@ -2891,12 +2891,12 @@
           <t>Time of Arrival</t>
         </is>
       </c>
-      <c r="AF4" s="11" t="inlineStr">
+      <c r="AF4" s="13" t="inlineStr">
         <is>
           <t>Tech</t>
         </is>
       </c>
-      <c r="AG4" s="12" t="inlineStr">
+      <c r="AG4" s="14" t="inlineStr">
         <is>
           <t>Time of Arrival</t>
         </is>
@@ -2970,8 +2970,16 @@
       <c r="AC5" s="17" t="n"/>
       <c r="AD5" s="16" t="n"/>
       <c r="AE5" s="17" t="n"/>
-      <c r="AF5" s="16" t="n"/>
-      <c r="AG5" s="17" t="n"/>
+      <c r="AF5" s="18" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AG5" s="19" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="21" r="6">
       <c r="A6" s="20" t="inlineStr">
@@ -3041,8 +3049,16 @@
       <c r="AC6" s="22" t="n"/>
       <c r="AD6" s="21" t="n"/>
       <c r="AE6" s="22" t="n"/>
-      <c r="AF6" s="21" t="n"/>
-      <c r="AG6" s="22" t="n"/>
+      <c r="AF6" s="23" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AG6" s="24" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="10" r="7">
       <c r="A7" s="10" t="n"/>
@@ -3076,8 +3092,8 @@
       <c r="AC7" s="26" t="n"/>
       <c r="AD7" s="25" t="n"/>
       <c r="AE7" s="26" t="n"/>
-      <c r="AF7" s="25" t="n"/>
-      <c r="AG7" s="26" t="n"/>
+      <c r="AF7" s="27" t="n"/>
+      <c r="AG7" s="28" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="8">
       <c r="A8" s="15" t="inlineStr">
@@ -3147,8 +3163,16 @@
       <c r="AC8" s="17" t="n"/>
       <c r="AD8" s="16" t="n"/>
       <c r="AE8" s="17" t="n"/>
-      <c r="AF8" s="16" t="n"/>
-      <c r="AG8" s="17" t="n"/>
+      <c r="AF8" s="18" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AG8" s="19" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="21" r="9">
       <c r="A9" s="20" t="inlineStr">
@@ -3218,8 +3242,16 @@
       <c r="AC9" s="22" t="n"/>
       <c r="AD9" s="21" t="n"/>
       <c r="AE9" s="22" t="n"/>
-      <c r="AF9" s="21" t="n"/>
-      <c r="AG9" s="22" t="n"/>
+      <c r="AF9" s="23" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AG9" s="24" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="10" r="10">
       <c r="A10" s="10" t="n"/>
@@ -3253,8 +3285,8 @@
       <c r="AC10" s="26" t="n"/>
       <c r="AD10" s="25" t="n"/>
       <c r="AE10" s="26" t="n"/>
-      <c r="AF10" s="25" t="n"/>
-      <c r="AG10" s="26" t="n"/>
+      <c r="AF10" s="27" t="n"/>
+      <c r="AG10" s="28" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="11">
       <c r="A11" s="15" t="inlineStr">
@@ -3324,8 +3356,16 @@
       <c r="AC11" s="17" t="n"/>
       <c r="AD11" s="16" t="n"/>
       <c r="AE11" s="17" t="n"/>
-      <c r="AF11" s="16" t="n"/>
-      <c r="AG11" s="17" t="n"/>
+      <c r="AF11" s="18" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AG11" s="19" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="21" r="12">
       <c r="A12" s="20" t="inlineStr">
@@ -3395,8 +3435,16 @@
       <c r="AC12" s="22" t="n"/>
       <c r="AD12" s="21" t="n"/>
       <c r="AE12" s="22" t="n"/>
-      <c r="AF12" s="21" t="n"/>
-      <c r="AG12" s="22" t="n"/>
+      <c r="AF12" s="23" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AG12" s="24" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="10" r="13">
       <c r="A13" s="10" t="n"/>
@@ -3430,8 +3478,8 @@
       <c r="AC13" s="26" t="n"/>
       <c r="AD13" s="25" t="n"/>
       <c r="AE13" s="26" t="n"/>
-      <c r="AF13" s="25" t="n"/>
-      <c r="AG13" s="26" t="n"/>
+      <c r="AF13" s="27" t="n"/>
+      <c r="AG13" s="28" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="14">
       <c r="A14" s="15" t="inlineStr">
@@ -3501,8 +3549,16 @@
       <c r="AC14" s="17" t="n"/>
       <c r="AD14" s="16" t="n"/>
       <c r="AE14" s="17" t="n"/>
-      <c r="AF14" s="16" t="n"/>
-      <c r="AG14" s="17" t="n"/>
+      <c r="AF14" s="18" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AG14" s="19" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="21" r="15">
       <c r="A15" s="20" t="inlineStr">
@@ -3572,8 +3628,16 @@
       <c r="AC15" s="22" t="n"/>
       <c r="AD15" s="21" t="n"/>
       <c r="AE15" s="22" t="n"/>
-      <c r="AF15" s="21" t="n"/>
-      <c r="AG15" s="22" t="n"/>
+      <c r="AF15" s="23" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AG15" s="24" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="10" r="16">
       <c r="A16" s="10" t="n"/>
@@ -3607,8 +3671,8 @@
       <c r="AC16" s="26" t="n"/>
       <c r="AD16" s="25" t="n"/>
       <c r="AE16" s="26" t="n"/>
-      <c r="AF16" s="25" t="n"/>
-      <c r="AG16" s="26" t="n"/>
+      <c r="AF16" s="27" t="n"/>
+      <c r="AG16" s="28" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="17">
       <c r="A17" s="15" t="inlineStr">
@@ -3678,8 +3742,16 @@
       <c r="AC17" s="17" t="n"/>
       <c r="AD17" s="16" t="n"/>
       <c r="AE17" s="17" t="n"/>
-      <c r="AF17" s="16" t="n"/>
-      <c r="AG17" s="17" t="n"/>
+      <c r="AF17" s="18" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AG17" s="19" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="21" r="18">
       <c r="A18" s="20" t="inlineStr">
@@ -3749,8 +3821,16 @@
       <c r="AC18" s="22" t="n"/>
       <c r="AD18" s="21" t="n"/>
       <c r="AE18" s="22" t="n"/>
-      <c r="AF18" s="21" t="n"/>
-      <c r="AG18" s="22" t="n"/>
+      <c r="AF18" s="23" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AG18" s="24" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="10" r="19">
       <c r="A19" s="10" t="n"/>
@@ -3784,8 +3864,8 @@
       <c r="AC19" s="26" t="n"/>
       <c r="AD19" s="25" t="n"/>
       <c r="AE19" s="26" t="n"/>
-      <c r="AF19" s="25" t="n"/>
-      <c r="AG19" s="26" t="n"/>
+      <c r="AF19" s="27" t="n"/>
+      <c r="AG19" s="28" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="20">
       <c r="A20" s="15" t="inlineStr">
@@ -3855,8 +3935,16 @@
       <c r="AC20" s="17" t="n"/>
       <c r="AD20" s="16" t="n"/>
       <c r="AE20" s="17" t="n"/>
-      <c r="AF20" s="16" t="n"/>
-      <c r="AG20" s="17" t="n"/>
+      <c r="AF20" s="18" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AG20" s="19" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="21" r="21">
       <c r="A21" s="20" t="inlineStr">
@@ -3926,8 +4014,16 @@
       <c r="AC21" s="22" t="n"/>
       <c r="AD21" s="21" t="n"/>
       <c r="AE21" s="22" t="n"/>
-      <c r="AF21" s="21" t="n"/>
-      <c r="AG21" s="22" t="n"/>
+      <c r="AF21" s="23" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AG21" s="24" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="10" r="22">
       <c r="A22" s="10" t="n"/>
@@ -3961,8 +4057,8 @@
       <c r="AC22" s="26" t="n"/>
       <c r="AD22" s="25" t="n"/>
       <c r="AE22" s="26" t="n"/>
-      <c r="AF22" s="25" t="n"/>
-      <c r="AG22" s="26" t="n"/>
+      <c r="AF22" s="27" t="n"/>
+      <c r="AG22" s="28" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="23">
       <c r="A23" s="15" t="inlineStr">
@@ -4032,8 +4128,16 @@
       <c r="AC23" s="17" t="n"/>
       <c r="AD23" s="16" t="n"/>
       <c r="AE23" s="17" t="n"/>
-      <c r="AF23" s="16" t="n"/>
-      <c r="AG23" s="17" t="n"/>
+      <c r="AF23" s="18" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AG23" s="19" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="21" r="24">
       <c r="A24" s="20" t="inlineStr">
@@ -4103,8 +4207,16 @@
       <c r="AC24" s="22" t="n"/>
       <c r="AD24" s="21" t="n"/>
       <c r="AE24" s="22" t="n"/>
-      <c r="AF24" s="21" t="n"/>
-      <c r="AG24" s="22" t="n"/>
+      <c r="AF24" s="23" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AG24" s="24" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="10" r="25">
       <c r="A25" s="10" t="n"/>
@@ -4138,8 +4250,8 @@
       <c r="AC25" s="26" t="n"/>
       <c r="AD25" s="25" t="n"/>
       <c r="AE25" s="26" t="n"/>
-      <c r="AF25" s="25" t="n"/>
-      <c r="AG25" s="26" t="n"/>
+      <c r="AF25" s="27" t="n"/>
+      <c r="AG25" s="28" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="26">
       <c r="A26" s="15" t="inlineStr">
@@ -4209,8 +4321,16 @@
       <c r="AC26" s="17" t="n"/>
       <c r="AD26" s="16" t="n"/>
       <c r="AE26" s="17" t="n"/>
-      <c r="AF26" s="16" t="n"/>
-      <c r="AG26" s="17" t="n"/>
+      <c r="AF26" s="18" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AG26" s="19" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="21" r="27">
       <c r="A27" s="9" t="inlineStr">
@@ -4280,8 +4400,16 @@
       <c r="AC27" s="30" t="n"/>
       <c r="AD27" s="29" t="n"/>
       <c r="AE27" s="30" t="n"/>
-      <c r="AF27" s="29" t="n"/>
-      <c r="AG27" s="30" t="n"/>
+      <c r="AF27" s="31" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AG27" s="32" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="33">

</xml_diff>